<commit_message>
save docs to pdf
</commit_message>
<xml_diff>
--- a/docs/PR - Deb FG Update Tempate How-To - in one.xlsx
+++ b/docs/PR - Deb FG Update Tempate How-To - in one.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Free Good Automation\Process Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\BR\zDev\US_Promo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B063856E-3AD5-472C-A3C2-540F8145B555}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -317,28 +318,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A3:G15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:G14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A2:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="4" name="ID" dataDxfId="8"/>
-    <tableColumn id="1" name="Field" dataDxfId="7"/>
-    <tableColumn id="2" name="Sample" dataDxfId="6"/>
-    <tableColumn id="3" name="Case 1:  buy X get X (@ item level; 3 Red pen + 1 Free Red)" dataDxfId="5"/>
-    <tableColumn id="7" name="Case 2:  buy X get Y (@ item level; 3 Red pen + 1 FreePencil)" dataDxfId="4"/>
-    <tableColumn id="6" name="Case 3:  buy X get X (@ Family set level; 1 Red + 1 Blue + 1 Black = 1 Free Blue)" dataDxfId="3"/>
-    <tableColumn id="5" name="Case 3:  buy X get Y  (@ Family set level; 1 Red + 1 Blue + 1 Black = Default or CSR choice)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Field" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sample" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Case 1:  buy X get X (@ item level; 3 Red pen + 1 Free Red)" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Case 2:  buy X get Y (@ item level; 3 Red pen + 1 FreePencil)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Case 3:  buy X get X (@ Family set level; 1 Red + 1 Blue + 1 Black = 1 Free Blue)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Case 3:  buy X get Y  (@ Family set level; 1 Red + 1 Blue + 1 Black = Default or CSR choice)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B21:D23" totalsRowShown="0">
-  <autoFilter ref="B21:D23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B18:D20" totalsRowShown="0">
+  <autoFilter ref="B18:D20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Detail Type" dataDxfId="1"/>
-    <tableColumn id="2" name="Item Select"/>
-    <tableColumn id="3" name="Family Set Select" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Detail Type" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Item Select"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Family Set Select" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,10 +607,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -620,119 +623,134 @@
     <col min="5" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" s="10" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4" t="s">
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="9" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>7770193</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>7770193</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
+      <c r="F5" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5">
+        <v>9</v>
+      </c>
       <c r="D6" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="C7" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4"/>
@@ -740,10 +758,10 @@
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
@@ -753,16 +771,18 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>7770193</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="4"/>
@@ -770,16 +790,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="5">
-        <v>7770193</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4"/>
@@ -787,31 +807,31 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>460165</v>
+      </c>
       <c r="D13" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
@@ -819,13 +839,13 @@
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5">
-        <v>460165</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>20</v>
@@ -834,66 +854,50 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+    <row r="18" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+    <row r="19" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="20" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>